<commit_message>
cambios en informacio financiera 2er trimestre 2022
</commit_message>
<xml_diff>
--- a/src/assets/content/estados-financieros/2022/tercer-trimestre/02_INFORMACION_PRESUPUESTARIA/02_ESTADO_ANALITICO_DE_EGRESOS_CLASIFICACION_ADMINISTRATIVA.xlsx
+++ b/src/assets/content/estados-financieros/2022/tercer-trimestre/02_INFORMACION_PRESUPUESTARIA/02_ESTADO_ANALITICO_DE_EGRESOS_CLASIFICACION_ADMINISTRATIVA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\2022\3.-3ER TRIMESTRE\INFORMACION FINANCIERA 3er trim\2.- INFORMACION PRESUPUESTARIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D295346A-7D93-4F3C-A139-9019B450464C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9689BD48-6305-471B-BD1D-37E340FDEF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E08E674F-14D4-4AC9-B75A-A59AC988CB69}"/>
   </bookViews>
@@ -409,8 +409,66 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -423,90 +481,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -833,793 +836,801 @@
   </sheetPr>
   <dimension ref="B2:I47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" style="4"/>
-    <col min="2" max="2" width="1.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="80.42578125" style="4" customWidth="1"/>
-    <col min="4" max="9" width="18.28515625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="12" style="4"/>
+    <col min="1" max="1" width="12" style="1"/>
+    <col min="2" max="2" width="1.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="80.42578125" style="1" customWidth="1"/>
+    <col min="4" max="9" width="18.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="12" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="7" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="28" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="29"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="3">
         <v>4</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="3">
         <v>5</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="18"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="9">
         <v>10302058.060000001</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="9">
         <v>1541821.76</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="9">
         <v>11843879.82</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="9">
         <v>7751184.0300000003</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="9">
         <v>7751184.0300000003</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="9">
         <v>4092695.79</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="18"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="9">
         <v>18751773.77</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="9">
         <v>3629871.19</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="9">
         <v>22381644.960000001</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="9">
         <v>15769621.039999999</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="9">
         <v>15769621.039999999</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="9">
         <v>6612023.9200000018</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="9">
         <v>17331036.620000001</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="9">
         <v>310364.27</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="9">
         <v>17641400.890000001</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="9">
         <v>10617263.02</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="9">
         <v>10617263.02</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="9">
         <v>7024137.870000001</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="9">
         <v>2606246.92</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="9">
         <v>615058.18999999994</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="9">
         <v>3221305.11</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="9">
         <v>2901907.32</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="9">
         <v>2901907.32</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="9">
         <v>319397.79000000004</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="9">
         <v>2960534.63</v>
       </c>
-      <c r="E11" s="20">
-        <v>0</v>
-      </c>
-      <c r="F11" s="20">
+      <c r="E11" s="9">
+        <v>0</v>
+      </c>
+      <c r="F11" s="9">
         <v>2960534.63</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="9">
         <v>1263780.49</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="9">
         <v>1263780.49</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="9">
         <v>1696754.14</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="20">
-        <v>0</v>
-      </c>
-      <c r="E12" s="20">
-        <v>0</v>
-      </c>
-      <c r="F12" s="20">
-        <v>0</v>
-      </c>
-      <c r="G12" s="20">
-        <v>0</v>
-      </c>
-      <c r="H12" s="20">
-        <v>0</v>
-      </c>
-      <c r="I12" s="20">
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0</v>
+      </c>
+      <c r="I12" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="20">
-        <v>0</v>
-      </c>
-      <c r="E13" s="20">
-        <v>0</v>
-      </c>
-      <c r="F13" s="20">
-        <v>0</v>
-      </c>
-      <c r="G13" s="20">
-        <v>0</v>
-      </c>
-      <c r="H13" s="20">
-        <v>0</v>
-      </c>
-      <c r="I13" s="20">
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="12">
         <v>51951650.000000007</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="12">
         <v>6097115.4100000001</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="12">
         <v>58048765.410000004</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="12">
         <v>38303755.900000006</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="12">
         <v>38303755.900000006</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="12">
         <v>19745009.510000002</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="1" t="s">
+      <c r="C19" s="23"/>
+      <c r="D19" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="7" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="28" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="11"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14">
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="3">
         <v>1</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="3">
         <v>2</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="3">
         <v>4</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="3">
         <v>5</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="18"/>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="20">
-        <v>0</v>
-      </c>
-      <c r="E22" s="20">
-        <v>0</v>
-      </c>
-      <c r="F22" s="20">
-        <v>0</v>
-      </c>
-      <c r="G22" s="20">
-        <v>0</v>
-      </c>
-      <c r="H22" s="20">
-        <v>0</v>
-      </c>
-      <c r="I22" s="20">
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="18"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="20">
-        <v>0</v>
-      </c>
-      <c r="E23" s="20">
-        <v>0</v>
-      </c>
-      <c r="F23" s="20">
-        <v>0</v>
-      </c>
-      <c r="G23" s="20">
-        <v>0</v>
-      </c>
-      <c r="H23" s="20">
-        <v>0</v>
-      </c>
-      <c r="I23" s="20">
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="18"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="20">
-        <v>0</v>
-      </c>
-      <c r="E24" s="20">
-        <v>0</v>
-      </c>
-      <c r="F24" s="20">
-        <v>0</v>
-      </c>
-      <c r="G24" s="20">
-        <v>0</v>
-      </c>
-      <c r="H24" s="20">
-        <v>0</v>
-      </c>
-      <c r="I24" s="20">
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="18"/>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="20">
-        <v>0</v>
-      </c>
-      <c r="E25" s="20">
-        <v>0</v>
-      </c>
-      <c r="F25" s="20">
-        <v>0</v>
-      </c>
-      <c r="G25" s="20">
-        <v>0</v>
-      </c>
-      <c r="H25" s="20">
-        <v>0</v>
-      </c>
-      <c r="I25" s="20">
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="21"/>
-      <c r="C26" s="22" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="23">
-        <v>0</v>
-      </c>
-      <c r="E26" s="23">
-        <v>0</v>
-      </c>
-      <c r="F26" s="23">
-        <v>0</v>
-      </c>
-      <c r="G26" s="23">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="23">
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="1" t="s">
+      <c r="C30" s="23"/>
+      <c r="D30" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="7" t="s">
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="28" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="11"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14">
+      <c r="B32" s="26"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="3">
         <v>1</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="3">
         <v>2</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="3">
         <v>4</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="3">
         <v>5</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="18"/>
-      <c r="C33" s="24" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="9">
         <v>51951650</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="9">
         <v>6097115.4100000001</v>
       </c>
-      <c r="F33" s="20">
+      <c r="F33" s="9">
         <v>58048765.409999996</v>
       </c>
-      <c r="G33" s="20">
+      <c r="G33" s="9">
         <v>38303755.899999999</v>
       </c>
-      <c r="H33" s="20">
+      <c r="H33" s="9">
         <v>38303755.899999999</v>
       </c>
-      <c r="I33" s="20">
+      <c r="I33" s="9">
         <v>19745009.509999998</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="18"/>
-      <c r="C34" s="24" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D34" s="20">
-        <v>0</v>
-      </c>
-      <c r="E34" s="20">
-        <v>0</v>
-      </c>
-      <c r="F34" s="20">
-        <v>0</v>
-      </c>
-      <c r="G34" s="20">
-        <v>0</v>
-      </c>
-      <c r="H34" s="20">
-        <v>0</v>
-      </c>
-      <c r="I34" s="20">
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0</v>
+      </c>
+      <c r="I34" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="18"/>
-      <c r="C35" s="24" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="20">
-        <v>0</v>
-      </c>
-      <c r="E35" s="20">
-        <v>0</v>
-      </c>
-      <c r="F35" s="20">
-        <v>0</v>
-      </c>
-      <c r="G35" s="20">
-        <v>0</v>
-      </c>
-      <c r="H35" s="20">
-        <v>0</v>
-      </c>
-      <c r="I35" s="20">
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+      <c r="I35" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="18"/>
-      <c r="C36" s="24" t="s">
+      <c r="B36" s="7"/>
+      <c r="C36" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="20">
-        <v>0</v>
-      </c>
-      <c r="E36" s="20">
-        <v>0</v>
-      </c>
-      <c r="F36" s="20">
-        <v>0</v>
-      </c>
-      <c r="G36" s="20">
-        <v>0</v>
-      </c>
-      <c r="H36" s="20">
-        <v>0</v>
-      </c>
-      <c r="I36" s="20">
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0</v>
+      </c>
+      <c r="I36" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="18"/>
-      <c r="C37" s="24" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="20">
-        <v>0</v>
-      </c>
-      <c r="E37" s="20">
-        <v>0</v>
-      </c>
-      <c r="F37" s="20">
-        <v>0</v>
-      </c>
-      <c r="G37" s="20">
-        <v>0</v>
-      </c>
-      <c r="H37" s="20">
-        <v>0</v>
-      </c>
-      <c r="I37" s="20">
+      <c r="D37" s="9">
+        <v>0</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0</v>
+      </c>
+      <c r="I37" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="18"/>
-      <c r="C38" s="24" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="20">
-        <v>0</v>
-      </c>
-      <c r="E38" s="20">
-        <v>0</v>
-      </c>
-      <c r="F38" s="20">
-        <v>0</v>
-      </c>
-      <c r="G38" s="20">
-        <v>0</v>
-      </c>
-      <c r="H38" s="20">
-        <v>0</v>
-      </c>
-      <c r="I38" s="20">
+      <c r="D38" s="9">
+        <v>0</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
+      <c r="G38" s="9">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0</v>
+      </c>
+      <c r="I38" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="18"/>
-      <c r="C39" s="24" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="20">
-        <v>0</v>
-      </c>
-      <c r="E39" s="20">
-        <v>0</v>
-      </c>
-      <c r="F39" s="20">
-        <v>0</v>
-      </c>
-      <c r="G39" s="20">
-        <v>0</v>
-      </c>
-      <c r="H39" s="20">
-        <v>0</v>
-      </c>
-      <c r="I39" s="20">
+      <c r="D39" s="9">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
+        <v>0</v>
+      </c>
+      <c r="F39" s="9">
+        <v>0</v>
+      </c>
+      <c r="G39" s="9">
+        <v>0</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0</v>
+      </c>
+      <c r="I39" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="21"/>
-      <c r="C40" s="22" t="s">
+      <c r="B40" s="10"/>
+      <c r="C40" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="23">
+      <c r="D40" s="12">
         <v>51951650</v>
       </c>
-      <c r="E40" s="23">
+      <c r="E40" s="12">
         <v>6097115.4100000001</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="12">
         <v>58048765.409999996</v>
       </c>
-      <c r="G40" s="23">
+      <c r="G40" s="12">
         <v>38303755.899999999</v>
       </c>
-      <c r="H40" s="23">
+      <c r="H40" s="12">
         <v>38303755.899999999</v>
       </c>
-      <c r="I40" s="23">
+      <c r="I40" s="12">
         <v>19745009.509999998</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="12" x14ac:dyDescent="0.2">
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27" t="s">
+      <c r="D45" s="15"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H45" s="27"/>
+      <c r="H45" s="30"/>
     </row>
     <row r="46" spans="2:9" ht="11.4" x14ac:dyDescent="0.2">
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29" t="s">
+      <c r="D46" s="15"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H46" s="29"/>
+      <c r="H46" s="18"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0" autoFilter="0"/>
   <mergeCells count="16">
+    <mergeCell ref="B19:C21"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B18:I18"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="B29:I29"/>
@@ -1628,14 +1639,6 @@
     <mergeCell ref="I30:I31"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:C21"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>